<commit_message>
Añadir destinatario adicional para el envío de reportes y crear nuevo reporte de tesorería
</commit_message>
<xml_diff>
--- a/reportes/reporte_extracciones_Técnica.xlsx
+++ b/reportes/reporte_extracciones_Técnica.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Reporte de novedades de máquinas en extracciones de dinero</t>
   </si>
@@ -31,22 +31,52 @@
     <t>Estado de Extracción</t>
   </si>
   <si>
-    <t>332830</t>
-  </si>
-  <si>
-    <t>480103</t>
-  </si>
-  <si>
-    <t>Llave limada</t>
+    <t>4000013</t>
+  </si>
+  <si>
+    <t>500104</t>
+  </si>
+  <si>
+    <t>Cerradura de Stacker Rota</t>
   </si>
   <si>
     <t>Pendiente</t>
   </si>
   <si>
-    <t>332832</t>
-  </si>
-  <si>
-    <t>422505</t>
+    <t>6000104</t>
+  </si>
+  <si>
+    <t>500101</t>
+  </si>
+  <si>
+    <t>Leva rota</t>
+  </si>
+  <si>
+    <t>Extraída</t>
+  </si>
+  <si>
+    <t>8002154</t>
+  </si>
+  <si>
+    <t>479906</t>
+  </si>
+  <si>
+    <t>8002153</t>
+  </si>
+  <si>
+    <t>479905</t>
+  </si>
+  <si>
+    <t>Puerta principal</t>
+  </si>
+  <si>
+    <t>8002150</t>
+  </si>
+  <si>
+    <t>479902</t>
+  </si>
+  <si>
+    <t>Puerta Belly</t>
   </si>
 </sst>
 </file>
@@ -109,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -119,6 +149,7 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="22" customWidth="1"/>
@@ -494,7 +525,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>45592.35196759259</v>
+        <v>45724.99804398148</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -510,20 +541,71 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>45592.35196759259</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5">
+        <v>45724.99804398148</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>45724.99804398148</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>45724.99804398148</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>45724.99804398148</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadir ruta y lógica para generar y enviar reporte diario
</commit_message>
<xml_diff>
--- a/reportes/reporte_extracciones_Técnica.xlsx
+++ b/reportes/reporte_extracciones_Técnica.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>Reporte de novedades de máquinas en extracciones de dinero</t>
   </si>
@@ -31,52 +31,146 @@
     <t>Estado de Extracción</t>
   </si>
   <si>
-    <t>4000013</t>
-  </si>
-  <si>
-    <t>500104</t>
-  </si>
-  <si>
-    <t>Cerradura de Stacker Rota</t>
+    <t>9000640</t>
+  </si>
+  <si>
+    <t>475206</t>
+  </si>
+  <si>
+    <t>Puerta3070 cerradura rota</t>
+  </si>
+  <si>
+    <t>Extraída</t>
+  </si>
+  <si>
+    <t>8001903</t>
+  </si>
+  <si>
+    <t>424102</t>
+  </si>
+  <si>
+    <t>Sin leva 901</t>
+  </si>
+  <si>
+    <t>10000139</t>
+  </si>
+  <si>
+    <t>480112</t>
+  </si>
+  <si>
+    <t>Sin leva 3070</t>
+  </si>
+  <si>
+    <t>8002433</t>
+  </si>
+  <si>
+    <t>107009</t>
+  </si>
+  <si>
+    <t>Falta de leva de stacker 901</t>
+  </si>
+  <si>
+    <t>8001083</t>
+  </si>
+  <si>
+    <t>459606</t>
+  </si>
+  <si>
+    <t>Zona 58 falta leva 901</t>
+  </si>
+  <si>
+    <t>8002154</t>
+  </si>
+  <si>
+    <t>479906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta leva de stakers </t>
+  </si>
+  <si>
+    <t>8001435</t>
+  </si>
+  <si>
+    <t>105502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerta principal abre sola </t>
+  </si>
+  <si>
+    <t>8001851</t>
+  </si>
+  <si>
+    <t>422704</t>
+  </si>
+  <si>
+    <t>Revisar llave número 20 no abre</t>
+  </si>
+  <si>
+    <t>8001673</t>
+  </si>
+  <si>
+    <t>308103</t>
+  </si>
+  <si>
+    <t>11000260</t>
+  </si>
+  <si>
+    <t>447605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin leva de stacker </t>
+  </si>
+  <si>
+    <t>7001449</t>
+  </si>
+  <si>
+    <t>302110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin leva 901
+</t>
+  </si>
+  <si>
+    <t>8001671</t>
+  </si>
+  <si>
+    <t>308101</t>
+  </si>
+  <si>
+    <t>9001005</t>
+  </si>
+  <si>
+    <t>105014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stacker sin leva </t>
+  </si>
+  <si>
+    <t>7000264</t>
+  </si>
+  <si>
+    <t>426502</t>
+  </si>
+  <si>
+    <t>Pta stacker rota se desarma</t>
+  </si>
+  <si>
+    <t>7000621</t>
+  </si>
+  <si>
+    <t>116204</t>
+  </si>
+  <si>
+    <t>Puerta principal</t>
   </si>
   <si>
     <t>Pendiente</t>
   </si>
   <si>
-    <t>6000104</t>
-  </si>
-  <si>
-    <t>500101</t>
-  </si>
-  <si>
-    <t>Leva rota</t>
-  </si>
-  <si>
-    <t>Extraída</t>
-  </si>
-  <si>
-    <t>8002154</t>
-  </si>
-  <si>
-    <t>479906</t>
-  </si>
-  <si>
-    <t>8002153</t>
-  </si>
-  <si>
-    <t>479905</t>
-  </si>
-  <si>
-    <t>Puerta principal</t>
-  </si>
-  <si>
-    <t>8002150</t>
-  </si>
-  <si>
-    <t>479902</t>
-  </si>
-  <si>
-    <t>Puerta Belly</t>
+    <t>1000008</t>
+  </si>
+  <si>
+    <t>463604</t>
   </si>
 </sst>
 </file>
@@ -147,9 +241,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,7 +583,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E20"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="22" customWidth="1"/>
@@ -525,24 +619,24 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>45724.99804398148</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>45724.99804398148</v>
+      <c r="A6" s="3">
+        <v>45732.44519675926</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -554,46 +648,46 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>45724.99804398148</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>45724.99804398148</v>
-      </c>
-      <c r="B8" s="4" t="s">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>45724.99804398148</v>
+      <c r="A9" s="3">
+        <v>45732.44519675926</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -605,7 +699,194 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>45732.44519675926</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`Removed email addresses from destinatariosTecnica, destinatariosZonas and destinatariosDiario arrays in enviarCorreoReporte function.`
</commit_message>
<xml_diff>
--- a/reportes/reporte_extracciones_Técnica.xlsx
+++ b/reportes/reporte_extracciones_Técnica.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Reporte de novedades de máquinas en extracciones de dinero</t>
   </si>
@@ -31,146 +31,99 @@
     <t>Estado de Extracción</t>
   </si>
   <si>
-    <t>9000640</t>
-  </si>
-  <si>
-    <t>475206</t>
-  </si>
-  <si>
-    <t>Puerta3070 cerradura rota</t>
+    <t>10000065</t>
+  </si>
+  <si>
+    <t>457603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No tiene código de barras para escanear </t>
   </si>
   <si>
     <t>Extraída</t>
   </si>
   <si>
-    <t>8001903</t>
-  </si>
-  <si>
-    <t>424102</t>
+    <t>9000466</t>
+  </si>
+  <si>
+    <t>421501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin leva 3070 z 56
+</t>
+  </si>
+  <si>
+    <t>8000653</t>
+  </si>
+  <si>
+    <t>423509</t>
+  </si>
+  <si>
+    <t>Cerradura de Stacker Rota</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>9000888</t>
+  </si>
+  <si>
+    <t>302708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amortiguadores y
+🚪 Puerta floja </t>
+  </si>
+  <si>
+    <t>9000099</t>
+  </si>
+  <si>
+    <t>100101</t>
+  </si>
+  <si>
+    <t>Puerta principal</t>
+  </si>
+  <si>
+    <t>10000445</t>
+  </si>
+  <si>
+    <t>448204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin leva de stacker </t>
+  </si>
+  <si>
+    <t>8000576</t>
+  </si>
+  <si>
+    <t>477505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta leva staker </t>
+  </si>
+  <si>
+    <t>8002154</t>
+  </si>
+  <si>
+    <t>479906</t>
+  </si>
+  <si>
+    <t>Sin leva</t>
+  </si>
+  <si>
+    <t>7000364</t>
+  </si>
+  <si>
+    <t>109402</t>
+  </si>
+  <si>
+    <t>3000036</t>
+  </si>
+  <si>
+    <t>465905</t>
   </si>
   <si>
     <t>Sin leva 901</t>
-  </si>
-  <si>
-    <t>10000139</t>
-  </si>
-  <si>
-    <t>480112</t>
-  </si>
-  <si>
-    <t>Sin leva 3070</t>
-  </si>
-  <si>
-    <t>8002433</t>
-  </si>
-  <si>
-    <t>107009</t>
-  </si>
-  <si>
-    <t>Falta de leva de stacker 901</t>
-  </si>
-  <si>
-    <t>8001083</t>
-  </si>
-  <si>
-    <t>459606</t>
-  </si>
-  <si>
-    <t>Zona 58 falta leva 901</t>
-  </si>
-  <si>
-    <t>8002154</t>
-  </si>
-  <si>
-    <t>479906</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falta leva de stakers </t>
-  </si>
-  <si>
-    <t>8001435</t>
-  </si>
-  <si>
-    <t>105502</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puerta principal abre sola </t>
-  </si>
-  <si>
-    <t>8001851</t>
-  </si>
-  <si>
-    <t>422704</t>
-  </si>
-  <si>
-    <t>Revisar llave número 20 no abre</t>
-  </si>
-  <si>
-    <t>8001673</t>
-  </si>
-  <si>
-    <t>308103</t>
-  </si>
-  <si>
-    <t>11000260</t>
-  </si>
-  <si>
-    <t>447605</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin leva de stacker </t>
-  </si>
-  <si>
-    <t>7001449</t>
-  </si>
-  <si>
-    <t>302110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin leva 901
-</t>
-  </si>
-  <si>
-    <t>8001671</t>
-  </si>
-  <si>
-    <t>308101</t>
-  </si>
-  <si>
-    <t>9001005</t>
-  </si>
-  <si>
-    <t>105014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stacker sin leva </t>
-  </si>
-  <si>
-    <t>7000264</t>
-  </si>
-  <si>
-    <t>426502</t>
-  </si>
-  <si>
-    <t>Pta stacker rota se desarma</t>
-  </si>
-  <si>
-    <t>7000621</t>
-  </si>
-  <si>
-    <t>116204</t>
-  </si>
-  <si>
-    <t>Puerta principal</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>1000008</t>
-  </si>
-  <si>
-    <t>463604</t>
   </si>
 </sst>
 </file>
@@ -583,7 +536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E14"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="22" customWidth="1"/>
@@ -619,7 +572,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>45732.44519675926</v>
+        <v>45734.49675925926</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -636,7 +589,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>45732.44519675926</v>
+        <v>45734.49675925926</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -652,68 +605,68 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>45732.44519675926</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="4">
+        <v>45734.49675925926</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>45732.44519675926</v>
+        <v>45734.49675925926</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>45732.44519675926</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="A9" s="4">
+        <v>45734.49675925926</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>45732.44519675926</v>
+        <v>45734.49675925926</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -721,16 +674,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>45732.44519675926</v>
+        <v>45734.49675925926</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -738,16 +691,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>45732.44519675926</v>
+        <v>45734.49675925926</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -755,16 +708,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>45732.44519675926</v>
+        <v>45734.49675925926</v>
       </c>
       <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -772,120 +725,18 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>45732.44519675926</v>
+        <v>45734.49675925926</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>45732.44519675926</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>45732.44519675926</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>45732.44519675926</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>45732.44519675926</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>45732.44519675926</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>45732.44519675926</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
`Added generateExcelExport function and updated routes to include Excel export functionality`
</commit_message>
<xml_diff>
--- a/reportes/reporte_extracciones_Técnica.xlsx
+++ b/reportes/reporte_extracciones_Técnica.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="93">
   <si>
     <t>Reporte de novedades de máquinas en extracciones de dinero</t>
   </si>
@@ -31,99 +31,268 @@
     <t>Estado de Extracción</t>
   </si>
   <si>
-    <t>10000065</t>
-  </si>
-  <si>
-    <t>457603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No tiene código de barras para escanear </t>
+    <t>8002080</t>
+  </si>
+  <si>
+    <t>305009</t>
+  </si>
+  <si>
+    <t>Puerta principal</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>8000362</t>
+  </si>
+  <si>
+    <t>107006</t>
+  </si>
+  <si>
+    <t>Cerradura de Stacker Rota</t>
+  </si>
+  <si>
+    <t>8001741</t>
+  </si>
+  <si>
+    <t>415404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin leva de stacker </t>
   </si>
   <si>
     <t>Extraída</t>
   </si>
   <si>
-    <t>9000466</t>
-  </si>
-  <si>
-    <t>421501</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin leva 3070 z 56
+    <t>9000983</t>
+  </si>
+  <si>
+    <t>471004</t>
+  </si>
+  <si>
+    <t>Se realizo extraccion</t>
+  </si>
+  <si>
+    <t>8001625</t>
+  </si>
+  <si>
+    <t>474905</t>
+  </si>
+  <si>
+    <t>Puerta principal rota</t>
+  </si>
+  <si>
+    <t>9000558</t>
+  </si>
+  <si>
+    <t>477608</t>
+  </si>
+  <si>
+    <t>No cierra puerta de stacker (3070) cerradura trabada</t>
+  </si>
+  <si>
+    <t>8001371</t>
+  </si>
+  <si>
+    <t>107501</t>
+  </si>
+  <si>
+    <t>Cerradura 20 abre sola</t>
+  </si>
+  <si>
+    <t>9000888</t>
+  </si>
+  <si>
+    <t>302708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerta principal rota, muy pesada corre riesgo que alguien se lastime. Se realizó extracción </t>
+  </si>
+  <si>
+    <t>7000851</t>
+  </si>
+  <si>
+    <t>100701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerta 3070 no abre nose realizo la extracción </t>
+  </si>
+  <si>
+    <t>7000274</t>
+  </si>
+  <si>
+    <t>426512</t>
+  </si>
+  <si>
+    <t>Puerta 20 no abre</t>
+  </si>
+  <si>
+    <t>7000854</t>
+  </si>
+  <si>
+    <t>100704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerta principal no abre se realizó extracción </t>
+  </si>
+  <si>
+    <t>7000269</t>
+  </si>
+  <si>
+    <t>426507</t>
+  </si>
+  <si>
+    <t>9001023</t>
+  </si>
+  <si>
+    <t>307505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerradura 020, falta tambor.
 </t>
   </si>
   <si>
-    <t>8000653</t>
-  </si>
-  <si>
-    <t>423509</t>
-  </si>
-  <si>
-    <t>Cerradura de Stacker Rota</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>9000888</t>
-  </si>
-  <si>
-    <t>302708</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amortiguadores y
-🚪 Puerta floja </t>
-  </si>
-  <si>
-    <t>9000099</t>
-  </si>
-  <si>
-    <t>100101</t>
-  </si>
-  <si>
-    <t>Puerta principal</t>
-  </si>
-  <si>
-    <t>10000445</t>
-  </si>
-  <si>
-    <t>448204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin leva de stacker </t>
-  </si>
-  <si>
-    <t>8000576</t>
-  </si>
-  <si>
-    <t>477505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falta leva staker </t>
-  </si>
-  <si>
-    <t>8002154</t>
-  </si>
-  <si>
-    <t>479906</t>
+    <t>9001014</t>
+  </si>
+  <si>
+    <t>108602</t>
+  </si>
+  <si>
+    <t>Sin leva 901</t>
+  </si>
+  <si>
+    <t>7000095</t>
+  </si>
+  <si>
+    <t>412705</t>
+  </si>
+  <si>
+    <t>Stacker leva mal armado 901</t>
+  </si>
+  <si>
+    <t>7000271</t>
+  </si>
+  <si>
+    <t>426509</t>
+  </si>
+  <si>
+    <t>9001020</t>
+  </si>
+  <si>
+    <t>307502</t>
+  </si>
+  <si>
+    <t>Falta pestillo apertura cerradura 020</t>
+  </si>
+  <si>
+    <t>9001021</t>
+  </si>
+  <si>
+    <t>307503</t>
+  </si>
+  <si>
+    <t>80000182</t>
+  </si>
+  <si>
+    <t>472701</t>
+  </si>
+  <si>
+    <t>Sin leva stacker</t>
+  </si>
+  <si>
+    <t>8002041</t>
+  </si>
+  <si>
+    <t>472101</t>
+  </si>
+  <si>
+    <t>Puerta principal rota queda abierta la maquina</t>
+  </si>
+  <si>
+    <t>10000260</t>
+  </si>
+  <si>
+    <t>447403</t>
+  </si>
+  <si>
+    <t>8001294</t>
+  </si>
+  <si>
+    <t>422104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerta principal no tiene tambor se abrio la segunda para extracción </t>
+  </si>
+  <si>
+    <t>7001677</t>
+  </si>
+  <si>
+    <t>473507</t>
+  </si>
+  <si>
+    <t>Puerta principal no cierra</t>
+  </si>
+  <si>
+    <t>7000196</t>
+  </si>
+  <si>
+    <t>426610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se encontró maquina abierta </t>
+  </si>
+  <si>
+    <t>8001671</t>
+  </si>
+  <si>
+    <t>308101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta leva stacker 901 </t>
+  </si>
+  <si>
+    <t>9000252</t>
+  </si>
+  <si>
+    <t>423608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falla de puerta accesoria abierta no funciona tactil para quitar falla
+</t>
+  </si>
+  <si>
+    <t>8002433</t>
+  </si>
+  <si>
+    <t>107009</t>
   </si>
   <si>
     <t>Sin leva</t>
   </si>
   <si>
-    <t>7000364</t>
-  </si>
-  <si>
-    <t>109402</t>
-  </si>
-  <si>
-    <t>3000036</t>
-  </si>
-  <si>
-    <t>465905</t>
-  </si>
-  <si>
-    <t>Sin leva 901</t>
+    <t>1000008</t>
+  </si>
+  <si>
+    <t>463604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta de leva de stacker </t>
+  </si>
+  <si>
+    <t>3000043</t>
+  </si>
+  <si>
+    <t>435201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin leva 901
+</t>
+  </si>
+  <si>
+    <t>3000026</t>
+  </si>
+  <si>
+    <t>435502</t>
   </si>
 </sst>
 </file>
@@ -194,9 +363,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +705,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E34"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="22" customWidth="1"/>
@@ -572,58 +741,58 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>45734.49675925926</v>
-      </c>
-      <c r="B5" t="s">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>45734.49675925926</v>
-      </c>
-      <c r="B6" t="s">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>45734.49675925926</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>45734.49675925926</v>
+      <c r="A8" s="5">
+        <v>45735.485243055555</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -635,29 +804,29 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>45734.49675925926</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>45734.49675925926</v>
+      <c r="A10" s="5">
+        <v>45735.485243055555</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -669,12 +838,12 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>45734.49675925926</v>
+      <c r="A11" s="5">
+        <v>45735.485243055555</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -686,12 +855,12 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>45734.49675925926</v>
+      <c r="A12" s="5">
+        <v>45735.485243055555</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -703,12 +872,12 @@
         <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>45734.49675925926</v>
+      <c r="A13" s="5">
+        <v>45735.485243055555</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
@@ -717,27 +886,367 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>45734.49675925926</v>
+      <c r="A14" s="5">
+        <v>45735.485243055555</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>45735.485243055555</v>
+      </c>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>